<commit_message>
created a table on postgres
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirleymalefane/Desktop/Basic-Queries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB002B89-E9D0-7C4A-A623-F15A49E125A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21447AEA-A74A-8142-99E2-6C7EFF929E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="8900" windowWidth="19800" windowHeight="16940" xr2:uid="{653BF5FA-01DB-4345-9926-BC3136A94AAB}"/>
+    <workbookView xWindow="2200" yWindow="4060" windowWidth="19800" windowHeight="16940" xr2:uid="{653BF5FA-01DB-4345-9926-BC3136A94AAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,359 +470,299 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7ACFC9-94BA-EF4C-A7D8-55BE5B185763}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+      <c r="D2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>154</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1009</v>
+      </c>
+      <c r="D4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>156</v>
+      </c>
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>0.02</v>
+      </c>
+      <c r="D6">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>159</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9999</v>
+      </c>
+      <c r="D8">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+      <c r="D9">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>161</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="D10">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>162</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>85</v>
+      </c>
+      <c r="D11">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>163</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>10021</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>153</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>43</v>
-      </c>
-      <c r="E2">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>154</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>70</v>
-      </c>
-      <c r="E3">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>155</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>1009</v>
-      </c>
-      <c r="E4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>156</v>
-      </c>
-      <c r="D5">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>165</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>166</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
         <v>53</v>
       </c>
-      <c r="E5">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>157</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>0.02</v>
-      </c>
-      <c r="E6">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>158</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>72</v>
-      </c>
-      <c r="E7">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>159</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>9999</v>
-      </c>
-      <c r="E8">
-        <v>2055</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>160</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D15">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>168</v>
+      </c>
+      <c r="B17" t="s">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>0.5</v>
-      </c>
-      <c r="E9">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>161</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>2009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>162</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>85</v>
-      </c>
-      <c r="E11">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>163</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>10021</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>164</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13">
-        <v>55</v>
-      </c>
-      <c r="E13">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>165</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14">
-        <v>45</v>
-      </c>
-      <c r="E14">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>166</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15">
-        <v>53</v>
-      </c>
-      <c r="E15">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>167</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16">
+      <c r="C17">
+        <v>2E-3</v>
+      </c>
+      <c r="D17">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>169</v>
+      </c>
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>170</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
         <v>49</v>
       </c>
-      <c r="E16">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>168</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>2E-3</v>
-      </c>
-      <c r="E17">
-        <v>2049</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>169</v>
-      </c>
-      <c r="D18">
-        <v>50</v>
-      </c>
-      <c r="E18">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>170</v>
-      </c>
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
       <c r="D19">
-        <v>49</v>
-      </c>
-      <c r="E19">
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>171</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>171</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
+      <c r="C20">
+        <v>9102</v>
       </c>
       <c r="D20">
-        <v>9102</v>
-      </c>
-      <c r="E20">
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>172</v>
+      </c>
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>172</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
+      <c r="C21">
+        <v>1E-3</v>
       </c>
       <c r="D21">
-        <v>1E-3</v>
-      </c>
-      <c r="E21">
         <v>9999</v>
       </c>
     </row>

</xml_diff>